<commit_message>
changes with the latest code for the create catalog page
</commit_message>
<xml_diff>
--- a/SellingoAutomations/Data/SellingoData.xlsx
+++ b/SellingoAutomations/Data/SellingoData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dk209\git\Sellingo\SellingoAutomations\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD9F915-6301-4350-A778-39FFC7B56F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF23DD9-52D6-4619-8CEB-00BDDCD6ADFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>MobileNumber</t>
   </si>
@@ -36,14 +36,185 @@
     <t>Test@123</t>
   </si>
   <si>
-    <t>9657803055</t>
+    <t>9307723916</t>
+  </si>
+  <si>
+    <t>Arraylist Headerlist1</t>
+  </si>
+  <si>
+    <t>Why sellingo?</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Tutorials</t>
+  </si>
+  <si>
+    <t>Pricing</t>
+  </si>
+  <si>
+    <t>Request Demo</t>
+  </si>
+  <si>
+    <t>FAQ</t>
+  </si>
+  <si>
+    <t>Arraylist Headerlist2</t>
+  </si>
+  <si>
+    <t>Arraylist Headerlist3</t>
+  </si>
+  <si>
+    <t>Arraylist Headerlist4</t>
+  </si>
+  <si>
+    <t>Arraylist Headerlist5</t>
+  </si>
+  <si>
+    <t>Arraylist Headerlist6</t>
+  </si>
+  <si>
+    <t>Expected Slide title Hashmap 1</t>
+  </si>
+  <si>
+    <t>Sell</t>
+  </si>
+  <si>
+    <t>Expected Slide title Hashmap 2</t>
+  </si>
+  <si>
+    <t>Expected Slide title Hashmap 3</t>
+  </si>
+  <si>
+    <t>Expected Slide title Hashmap 4</t>
+  </si>
+  <si>
+    <t>Expected Slide title Hashmap 5</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Share</t>
+  </si>
+  <si>
+    <t>Track</t>
+  </si>
+  <si>
+    <t>Increase Sales</t>
+  </si>
+  <si>
+    <t>Expected Slide Subtitle Hashmap 1</t>
+  </si>
+  <si>
+    <t>Your Product in 2 minutes</t>
+  </si>
+  <si>
+    <t>Your Online Store</t>
+  </si>
+  <si>
+    <t>Catalog On The Go</t>
+  </si>
+  <si>
+    <t>Customer's Activity</t>
+  </si>
+  <si>
+    <t>By Getting Quick Orders</t>
+  </si>
+  <si>
+    <t>Expected Slide Subtitle Hashmap 2</t>
+  </si>
+  <si>
+    <t>Expected Slide Subtitle Hashmap 3</t>
+  </si>
+  <si>
+    <t>Expected Slide Subtitle Hashmap 4</t>
+  </si>
+  <si>
+    <t>Expected Slide Subtitle Hashmap 5</t>
+  </si>
+  <si>
+    <t>expectedRegiterText</t>
+  </si>
+  <si>
+    <t>REGISTER</t>
+  </si>
+  <si>
+    <t>expectedLoginText</t>
+  </si>
+  <si>
+    <t>LOGIN</t>
+  </si>
+  <si>
+    <t>expectedFacebookURL</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/SellingoOnlineStore</t>
+  </si>
+  <si>
+    <t>x.com</t>
+  </si>
+  <si>
+    <t>TwitterURL</t>
+  </si>
+  <si>
+    <t>expectedInstagramURL</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/sellingo_onlinestore/</t>
+  </si>
+  <si>
+    <t>linkedin.com</t>
+  </si>
+  <si>
+    <t>LinkedinURL</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCSoIdbOJxMmgPe1cm_L6nww</t>
+  </si>
+  <si>
+    <t>expctedYouTubeURL</t>
+  </si>
+  <si>
+    <t>expectedMobileNumberErrorMessage</t>
+  </si>
+  <si>
+    <t>Mobile Number is required</t>
+  </si>
+  <si>
+    <t>expectedPasswordErrorMessage</t>
+  </si>
+  <si>
+    <t>Password is required</t>
+  </si>
+  <si>
+    <t>expectedErrorMessage</t>
+  </si>
+  <si>
+    <t>Please enter mobile number.</t>
+  </si>
+  <si>
+    <t>OTP is required</t>
+  </si>
+  <si>
+    <t>expectedErrorMessageOTP</t>
+  </si>
+  <si>
+    <t>expectedErrorMessageforgotPass</t>
+  </si>
+  <si>
+    <t>expectedLoggedInUrl</t>
+  </si>
+  <si>
+    <t>https://www.sellingo.ai/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +229,31 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF6A3E3E"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0066CC"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,10 +277,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -366,16 +565,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="48.44140625" customWidth="1"/>
+    <col min="2" max="2" width="77.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -394,10 +593,244 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{127D5061-28AB-472B-88A7-34170DA59484}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
latest code for running test cases in a single run
</commit_message>
<xml_diff>
--- a/SellingoAutomations/Data/SellingoData.xlsx
+++ b/SellingoAutomations/Data/SellingoData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dk209\git\Sellingo\SellingoAutomations\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF23DD9-52D6-4619-8CEB-00BDDCD6ADFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54D6AB9-C1FF-4901-8959-B23D6B63A2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>MobileNumber</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Test@123</t>
   </si>
   <si>
-    <t>9307723916</t>
-  </si>
-  <si>
     <t>Arraylist Headerlist1</t>
   </si>
   <si>
@@ -171,50 +168,89 @@
     <t>LinkedinURL</t>
   </si>
   <si>
+    <t>expctedYouTubeURL</t>
+  </si>
+  <si>
+    <t>expectedMobileNumberErrorMessage</t>
+  </si>
+  <si>
+    <t>Mobile Number is required</t>
+  </si>
+  <si>
+    <t>expectedPasswordErrorMessage</t>
+  </si>
+  <si>
+    <t>Password is required</t>
+  </si>
+  <si>
+    <t>expectedErrorMessage</t>
+  </si>
+  <si>
+    <t>Please enter mobile number.</t>
+  </si>
+  <si>
+    <t>OTP is required</t>
+  </si>
+  <si>
+    <t>expectedErrorMessageOTP</t>
+  </si>
+  <si>
+    <t>expectedErrorMessageforgotPass</t>
+  </si>
+  <si>
+    <t>expectedLoggedInUrl</t>
+  </si>
+  <si>
+    <t>https://www.sellingo.ai/</t>
+  </si>
+  <si>
+    <t>CatalogName</t>
+  </si>
+  <si>
+    <t>TestCatalogName2</t>
+  </si>
+  <si>
+    <t>catalog image</t>
+  </si>
+  <si>
+    <t>C:\\Users\\dk209\\Downloads\\Narrow Chain Bracelet &amp; Plain Bangle - Narrow Chain Bracelet &amp;amp; Plain Bangle.jpeg</t>
+  </si>
+  <si>
+    <t>CatalogDescription</t>
+  </si>
+  <si>
+    <t>Test Catalog Description</t>
+  </si>
+  <si>
+    <t>Add to Cart</t>
+  </si>
+  <si>
+    <t>dropdown values</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/channel/UCSoIdbOJxMmgPe1cm_L6nww</t>
   </si>
   <si>
-    <t>expctedYouTubeURL</t>
-  </si>
-  <si>
-    <t>expectedMobileNumberErrorMessage</t>
-  </si>
-  <si>
-    <t>Mobile Number is required</t>
-  </si>
-  <si>
-    <t>expectedPasswordErrorMessage</t>
-  </si>
-  <si>
-    <t>Password is required</t>
-  </si>
-  <si>
-    <t>expectedErrorMessage</t>
-  </si>
-  <si>
-    <t>Please enter mobile number.</t>
-  </si>
-  <si>
-    <t>OTP is required</t>
-  </si>
-  <si>
-    <t>expectedErrorMessageOTP</t>
-  </si>
-  <si>
-    <t>expectedErrorMessageforgotPass</t>
-  </si>
-  <si>
-    <t>expectedLoggedInUrl</t>
-  </si>
-  <si>
-    <t>https://www.sellingo.ai/</t>
+    <t>Forgot Password Text</t>
+  </si>
+  <si>
+    <t>Forgot Password</t>
+  </si>
+  <si>
+    <t>SuccessOtp message</t>
+  </si>
+  <si>
+    <t>OTP has been sent successfully.</t>
+  </si>
+  <si>
+    <t>9657803055</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,29 +267,68 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF2A00FF"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF6A3E3E"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF0066CC"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF221A15"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -277,13 +352,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -565,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,259 +657,308 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="3" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="3" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="3" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="3" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="B23" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="5" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="B25" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="B31" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>60</v>
       </c>
     </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{127D5061-28AB-472B-88A7-34170DA59484}"/>
+    <hyperlink ref="B25" r:id="rId2" xr:uid="{76644B06-5B74-43FA-B61A-F703DE7CD4E7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final push with 20 Test cases
</commit_message>
<xml_diff>
--- a/SellingoAutomations/Data/SellingoData.xlsx
+++ b/SellingoAutomations/Data/SellingoData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dk209\git\Sellingo\SellingoAutomations\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54D6AB9-C1FF-4901-8959-B23D6B63A2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9481A6-06EE-44BA-BF56-01C883F88D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
   <si>
     <t>MobileNumber</t>
   </si>
@@ -207,9 +207,6 @@
     <t>CatalogName</t>
   </si>
   <si>
-    <t>TestCatalogName2</t>
-  </si>
-  <si>
     <t>catalog image</t>
   </si>
   <si>
@@ -243,14 +240,44 @@
     <t>OTP has been sent successfully.</t>
   </si>
   <si>
-    <t>9657803055</t>
+    <t>7757810088</t>
+  </si>
+  <si>
+    <t>Text on Enquiry Button</t>
+  </si>
+  <si>
+    <t>Step2 text</t>
+  </si>
+  <si>
+    <t>PUBLISH CATALOG</t>
+  </si>
+  <si>
+    <t>Publish Catalog Step 3 text</t>
+  </si>
+  <si>
+    <t>Total views Text</t>
+  </si>
+  <si>
+    <t>CatalogNameEdit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Catalog Description Edit </t>
+  </si>
+  <si>
+    <t>Test Catalog Name 123</t>
+  </si>
+  <si>
+    <t>Tes tCatalog Name New</t>
+  </si>
+  <si>
+    <t>Total Views:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,6 +356,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF221A15"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000C0"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -352,7 +397,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -363,6 +408,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -644,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -661,7 +711,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -853,7 +903,7 @@
         <v>47</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -909,47 +959,87 @@
         <v>59</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>71</v>
+    </row>
+    <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>